<commit_message>
edit a student function
</commit_message>
<xml_diff>
--- a/planner.xlsx
+++ b/planner.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4602D472-35DA-40DF-8C66-4F369D0DA507}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E578249-A2E9-9A4C-94A0-8DEDB5C4C92F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1249,14 +1247,14 @@
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Bình thường" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Đầu đề 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -1494,15 +1492,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>63500</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>15</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1790,16 +1788,16 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.875" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="52.125" customWidth="1"/>
-    <col min="4" max="4" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="52.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
     <col min="5" max="5" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="69" t="s">
         <v>14</v>
       </c>
@@ -1811,7 +1809,7 @@
       <c r="G1" s="69"/>
       <c r="H1" s="69"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="69"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -1821,7 +1819,7 @@
       <c r="G2" s="69"/>
       <c r="H2" s="69"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
       <c r="B3" s="69"/>
       <c r="C3" s="69"/>
@@ -1831,7 +1829,7 @@
       <c r="G3" s="69"/>
       <c r="H3" s="69"/>
     </row>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>32</v>
       </c>
@@ -1839,7 +1837,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>33</v>
       </c>
@@ -1847,7 +1845,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
@@ -1855,7 +1853,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>15</v>
       </c>
@@ -1872,7 +1870,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="23" t="s">
         <v>17</v>
       </c>
@@ -1883,7 +1881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>18</v>
       </c>
@@ -1894,7 +1892,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
         <v>19</v>
       </c>
@@ -1904,7 +1902,7 @@
       <c r="E13" s="27"/>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>20</v>
       </c>
@@ -1913,7 +1911,7 @@
       </c>
       <c r="F14" s="26"/>
     </row>
-    <row r="15" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>21</v>
       </c>
@@ -1921,7 +1919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>22</v>
       </c>
@@ -1949,15 +1947,15 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.625" customWidth="1"/>
-    <col min="3" max="3" width="27.75" customWidth="1"/>
-    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="69" t="s">
         <v>34</v>
       </c>
@@ -1967,7 +1965,7 @@
       <c r="E1" s="69"/>
       <c r="F1" s="69"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="69"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -1975,7 +1973,7 @@
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
     </row>
-    <row r="3" spans="1:6" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
       <c r="B3" s="69"/>
       <c r="C3" s="69"/>
@@ -1983,7 +1981,7 @@
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="17" t="s">
         <v>35</v>
       </c>
@@ -1991,10 +1989,10 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="17" t="s">
         <v>36</v>
       </c>
@@ -2008,7 +2006,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="17"/>
       <c r="C7" s="67" t="s">
         <v>99</v>
@@ -2020,7 +2018,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="17"/>
       <c r="C8" s="67" t="s">
         <v>100</v>
@@ -2032,7 +2030,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="17"/>
       <c r="C9" s="67" t="s">
         <v>101</v>
@@ -2044,7 +2042,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="17"/>
       <c r="C10" s="67" t="s">
         <v>102</v>
@@ -2056,16 +2054,16 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="17"/>
       <c r="C11" s="67"/>
       <c r="D11" s="68"/>
       <c r="E11" s="67"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>37</v>
       </c>
@@ -2076,7 +2074,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="s">
         <v>38</v>
       </c>
@@ -2085,41 +2083,41 @@
       </c>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="17"/>
       <c r="C15" s="28"/>
     </row>
-    <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.2">
       <c r="C21" s="50" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C22" s="46" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C23" s="46" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C24" s="46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C25" s="46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" ht="29" x14ac:dyDescent="0.2">
       <c r="C27" s="54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" ht="29" x14ac:dyDescent="0.2">
       <c r="C28" s="54" t="s">
         <v>97</v>
       </c>
@@ -2152,45 +2150,45 @@
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="40" customWidth="1"/>
-    <col min="2" max="2" width="41.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="4.125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="2.875" style="1"/>
+    <col min="11" max="11" width="5.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="2.83203125" style="1"/>
     <col min="13" max="13" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="8" style="1" customWidth="1"/>
     <col min="18" max="18" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="2.875" style="1"/>
-    <col min="23" max="23" width="3.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.625" style="1" customWidth="1"/>
-    <col min="25" max="29" width="2.875" style="1"/>
+    <col min="19" max="22" width="2.83203125" style="1"/>
+    <col min="23" max="23" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.6640625" style="1" customWidth="1"/>
+    <col min="25" max="29" width="2.83203125" style="1"/>
     <col min="30" max="30" width="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="8.5" customWidth="1"/>
-    <col min="37" max="37" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.125" customWidth="1"/>
-    <col min="44" max="44" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.1640625" customWidth="1"/>
+    <col min="44" max="44" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
@@ -2201,7 +2199,7 @@
       <c r="G1" s="70"/>
       <c r="H1" s="70"/>
     </row>
-    <row r="2" spans="1:66" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -2245,7 +2243,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="70"/>
       <c r="C3" s="70"/>
       <c r="D3" s="70"/>
@@ -2259,7 +2257,7 @@
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
     </row>
-    <row r="4" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="32" t="s">
@@ -2702,7 +2700,7 @@
       <c r="BM7" s="3"/>
       <c r="BN7" s="3"/>
     </row>
-    <row r="8" spans="1:66" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A8" s="64">
         <v>1</v>
       </c>
@@ -2716,7 +2714,7 @@
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="65">
         <v>1.1000000000000001</v>
       </c>
@@ -2742,7 +2740,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="65">
         <v>1.2</v>
       </c>
@@ -2762,7 +2760,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="65">
         <v>1.3</v>
       </c>
@@ -2782,7 +2780,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="65">
         <v>1.4</v>
       </c>
@@ -2802,7 +2800,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="65">
         <v>1.5</v>
       </c>
@@ -2818,17 +2816,11 @@
       <c r="E13" s="14">
         <v>14</v>
       </c>
-      <c r="F13" s="14">
-        <v>2</v>
-      </c>
-      <c r="G13" s="14">
-        <v>1</v>
-      </c>
-      <c r="H13" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:66" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A14" s="64">
         <v>2</v>
       </c>
@@ -2842,7 +2834,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="65">
         <v>2.1</v>
       </c>
@@ -2862,7 +2854,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:66" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" s="52" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="66">
         <v>2.2000000000000002</v>
       </c>
@@ -2903,7 +2895,7 @@
       <c r="AB16" s="57"/>
       <c r="AC16" s="57"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="65">
         <v>2.2999999999999998</v>
       </c>
@@ -2919,11 +2911,17 @@
       <c r="E17" s="14">
         <v>14</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F17" s="14">
+        <v>2</v>
+      </c>
+      <c r="G17" s="14">
+        <v>1</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="65">
         <v>2.4</v>
       </c>
@@ -2943,7 +2941,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="65">
         <v>2.5</v>
       </c>
@@ -2963,7 +2961,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="15"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="65">
         <v>2.6</v>
       </c>
@@ -2983,7 +2981,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="65">
         <v>2.7</v>
       </c>
@@ -3003,7 +3001,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="64">
         <v>3</v>
       </c>
@@ -3017,7 +3015,7 @@
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="65">
         <v>3.1</v>
       </c>
@@ -3031,7 +3029,7 @@
       <c r="G23" s="14"/>
       <c r="H23" s="15"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="65">
         <v>3.2</v>
       </c>
@@ -3045,7 +3043,7 @@
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="65">
         <v>3.3</v>
       </c>
@@ -3059,7 +3057,7 @@
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="65">
         <v>3.4</v>
       </c>
@@ -3073,7 +3071,7 @@
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="65">
         <v>3.5</v>
       </c>
@@ -3087,7 +3085,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="65">
         <v>3.6</v>
       </c>
@@ -3101,7 +3099,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="65">
         <v>3.7</v>
       </c>
@@ -3115,7 +3113,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="65">
         <v>3.8</v>
       </c>
@@ -3129,7 +3127,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="65">
         <v>3.9</v>
       </c>
@@ -3143,7 +3141,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="65" t="s">
         <v>110</v>
       </c>
@@ -3157,7 +3155,7 @@
       <c r="G32" s="14"/>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="65">
         <v>3.11</v>
       </c>
@@ -3171,7 +3169,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="64">
         <v>4</v>
       </c>
@@ -3185,7 +3183,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="65">
         <v>4.0999999999999996</v>
       </c>
@@ -3199,7 +3197,7 @@
       <c r="G35" s="14"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="65">
         <v>4.2</v>
       </c>
@@ -3213,7 +3211,7 @@
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="64">
         <v>5</v>
       </c>
@@ -3227,7 +3225,7 @@
       <c r="G37" s="14"/>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="65">
         <v>5.0999999999999996</v>
       </c>
@@ -3241,7 +3239,7 @@
       <c r="G38" s="14"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="65">
         <v>5.2</v>
       </c>
@@ -3255,7 +3253,7 @@
       <c r="G39" s="14"/>
       <c r="H39" s="15"/>
     </row>
-    <row r="40" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="64">
         <v>6</v>
       </c>
@@ -3269,7 +3267,7 @@
       <c r="G40" s="14"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="65">
         <v>6.1</v>
       </c>
@@ -3283,7 +3281,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="15"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="65">
         <v>6.2</v>
       </c>
@@ -3297,7 +3295,7 @@
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="65">
         <v>6.3</v>
       </c>
@@ -3311,7 +3309,7 @@
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="65">
         <v>6.4</v>
       </c>
@@ -3325,7 +3323,7 @@
       <c r="G44" s="14"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="65">
         <v>6.5</v>
       </c>
@@ -3339,7 +3337,7 @@
       <c r="G45" s="14"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="65">
         <v>6.6</v>
       </c>
@@ -3353,7 +3351,7 @@
       <c r="G46" s="14"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="65">
         <v>6.7</v>
       </c>
@@ -3367,7 +3365,7 @@
       <c r="G47" s="14"/>
       <c r="H47" s="15"/>
     </row>
-    <row r="48" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="64">
         <v>7</v>
       </c>
@@ -3381,7 +3379,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="65">
         <v>7.1</v>
       </c>
@@ -3395,7 +3393,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="65">
         <v>7.2</v>
       </c>
@@ -3409,7 +3407,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="65">
         <v>7.3</v>
       </c>
@@ -3423,7 +3421,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="15"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="65">
         <v>7.4</v>
       </c>
@@ -3437,7 +3435,7 @@
       <c r="G52" s="14"/>
       <c r="H52" s="15"/>
     </row>
-    <row r="53" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="64" t="s">
         <v>127</v>
       </c>
@@ -3451,7 +3449,7 @@
       <c r="G53" s="14"/>
       <c r="H53" s="15"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="65" t="s">
         <v>129</v>
       </c>
@@ -3465,7 +3463,7 @@
       <c r="G54" s="14"/>
       <c r="H54" s="15"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="65"/>
       <c r="B55" s="62"/>
       <c r="C55" s="58"/>
@@ -3475,7 +3473,7 @@
       <c r="G55" s="14"/>
       <c r="H55" s="15"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="65"/>
       <c r="B56" s="62"/>
       <c r="C56" s="58"/>
@@ -3485,7 +3483,7 @@
       <c r="G56" s="14"/>
       <c r="H56" s="15"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="65"/>
       <c r="B57" s="62"/>
       <c r="C57" s="58"/>
@@ -3495,7 +3493,7 @@
       <c r="G57" s="14"/>
       <c r="H57" s="15"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="65"/>
       <c r="B58" s="62"/>
       <c r="C58" s="58"/>
@@ -3505,7 +3503,7 @@
       <c r="G58" s="14"/>
       <c r="H58" s="15"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="65"/>
       <c r="B59" s="62"/>
       <c r="C59" s="58"/>
@@ -3515,7 +3513,7 @@
       <c r="G59" s="14"/>
       <c r="H59" s="15"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="65"/>
       <c r="B60" s="62"/>
       <c r="C60" s="58"/>
@@ -3525,26 +3523,26 @@
       <c r="G60" s="14"/>
       <c r="H60" s="15"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="41"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="41"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="41"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>53</v>
       </c>
@@ -3607,15 +3605,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>15</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:colOff>63500</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>15</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3644,14 +3642,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.875" customWidth="1"/>
-    <col min="2" max="2" width="125.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="125.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
         <v>45</v>
       </c>
@@ -3662,7 +3660,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="52" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="51">
         <v>1.1000000000000001</v>
       </c>
@@ -3671,44 +3669,44 @@
       </c>
       <c r="C3" s="51"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
       <c r="B4" s="47"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="47"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
       <c r="B6" s="47"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="47"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="48"/>
       <c r="B8" s="47"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="47"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="48"/>
       <c r="B10" s="47"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="48"/>
       <c r="B11" s="47"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="48"/>
       <c r="B12" s="47"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="42"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add change pw function
</commit_message>
<xml_diff>
--- a/planner.xlsx
+++ b/planner.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD4BF40-B306-4229-AFD6-72D6341DE240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E482FA-18FC-47D6-8969-DE277AB24D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2152,7 +2152,7 @@
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2784,9 +2784,15 @@
       <c r="E12" s="14">
         <v>14</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="F12" s="14">
+        <v>3</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A13" s="65">

</xml_diff>

<commit_message>
split menu into a separated file
</commit_message>
<xml_diff>
--- a/planner.xlsx
+++ b/planner.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E482FA-18FC-47D6-8969-DE277AB24D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4D85D7-9E11-4BC4-B040-85DFBE424218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="134">
   <si>
     <t>Project Planner</t>
   </si>
@@ -596,6 +596,12 @@
   </si>
   <si>
     <t>Staff login done (1/3)</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Settings</t>
   </si>
 </sst>
 </file>
@@ -2145,14 +2151,14 @@
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN89"/>
+  <dimension ref="A1:BN68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="6" topLeftCell="J52" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2716,7 +2722,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="15">
         <v>0.33</v>
@@ -3464,8 +3470,12 @@
       <c r="H54" s="15"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="65"/>
-      <c r="B55" s="62"/>
+      <c r="A55" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="62" t="s">
+        <v>133</v>
+      </c>
       <c r="C55" s="58"/>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
@@ -3532,18 +3542,18 @@
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="41"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B87" s="2" t="s">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B88" s="2" t="s">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B89" s="2" t="s">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="2" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sửa lại, sử dụng list
</commit_message>
<xml_diff>
--- a/planner.xlsx
+++ b/planner.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4D85D7-9E11-4BC4-B040-85DFBE424218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BEEAAC-8D36-DB47-A753-94BD184B557B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -1255,14 +1255,14 @@
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Bình thường" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Đầu đề 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -1500,15 +1500,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>63500</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>15</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1796,16 +1796,16 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.875" customWidth="1"/>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="52.125" customWidth="1"/>
-    <col min="4" max="4" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="52.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
     <col min="5" max="5" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="69" t="s">
         <v>14</v>
       </c>
@@ -1817,7 +1817,7 @@
       <c r="G1" s="69"/>
       <c r="H1" s="69"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="69"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -1827,7 +1827,7 @@
       <c r="G2" s="69"/>
       <c r="H2" s="69"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
       <c r="B3" s="69"/>
       <c r="C3" s="69"/>
@@ -1837,7 +1837,7 @@
       <c r="G3" s="69"/>
       <c r="H3" s="69"/>
     </row>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>32</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>33</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>15</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="23" t="s">
         <v>17</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="23" t="s">
         <v>18</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="23" t="s">
         <v>19</v>
       </c>
@@ -1910,7 +1910,7 @@
       <c r="E13" s="27"/>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="23" t="s">
         <v>20</v>
       </c>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="F14" s="26"/>
     </row>
-    <row r="15" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
         <v>21</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>22</v>
       </c>
@@ -1955,15 +1955,15 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.625" customWidth="1"/>
-    <col min="3" max="3" width="27.625" customWidth="1"/>
-    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
     <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="69" t="s">
         <v>34</v>
       </c>
@@ -1973,7 +1973,7 @@
       <c r="E1" s="69"/>
       <c r="F1" s="69"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="69"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -1981,7 +1981,7 @@
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
     </row>
-    <row r="3" spans="1:6" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
       <c r="B3" s="69"/>
       <c r="C3" s="69"/>
@@ -1989,7 +1989,7 @@
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="17" t="s">
         <v>35</v>
       </c>
@@ -1997,10 +1997,10 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="17" t="s">
         <v>36</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="17"/>
       <c r="C7" s="67" t="s">
         <v>99</v>
@@ -2026,7 +2026,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="17"/>
       <c r="C8" s="67" t="s">
         <v>100</v>
@@ -2038,7 +2038,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="17"/>
       <c r="C9" s="67" t="s">
         <v>101</v>
@@ -2050,7 +2050,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="17"/>
       <c r="C10" s="67" t="s">
         <v>102</v>
@@ -2062,16 +2062,16 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="17"/>
       <c r="C11" s="67"/>
       <c r="D11" s="68"/>
       <c r="E11" s="67"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>37</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="s">
         <v>38</v>
       </c>
@@ -2091,41 +2091,41 @@
       </c>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="17"/>
       <c r="C15" s="28"/>
     </row>
-    <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.2">
       <c r="C21" s="50" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C22" s="46" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C23" s="46" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C24" s="46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" ht="16" x14ac:dyDescent="0.2">
       <c r="C25" s="46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" ht="29" x14ac:dyDescent="0.2">
       <c r="C27" s="54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" ht="29" x14ac:dyDescent="0.2">
       <c r="C28" s="54" t="s">
         <v>97</v>
       </c>
@@ -2153,30 +2153,30 @@
   </sheetPr>
   <dimension ref="A1:BN68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="6" topLeftCell="J52" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="9" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="40" customWidth="1"/>
-    <col min="2" max="2" width="41.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="4.125" style="1" customWidth="1"/>
-    <col min="10" max="29" width="7.625" style="1" customWidth="1"/>
-    <col min="30" max="66" width="7.625" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" style="1" customWidth="1"/>
+    <col min="10" max="29" width="7.6640625" style="1" customWidth="1"/>
+    <col min="30" max="66" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="G1" s="70"/>
       <c r="H1" s="70"/>
     </row>
-    <row r="2" spans="1:66" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -2231,7 +2231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="70"/>
       <c r="C3" s="70"/>
       <c r="D3" s="70"/>
@@ -2245,7 +2245,7 @@
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
     </row>
-    <row r="4" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="32" t="s">
@@ -2688,7 +2688,7 @@
       <c r="BM7" s="3"/>
       <c r="BN7" s="3"/>
     </row>
-    <row r="8" spans="1:66" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A8" s="64">
         <v>1</v>
       </c>
@@ -2702,7 +2702,7 @@
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="65">
         <v>1.1000000000000001</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="65">
         <v>1.2</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="65">
         <v>1.3</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="65">
         <v>1.4</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="65">
         <v>1.5</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:66" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A14" s="64">
         <v>2</v>
       </c>
@@ -2840,7 +2840,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="65">
         <v>2.1</v>
       </c>
@@ -2860,7 +2860,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:66" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" s="52" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="66">
         <v>2.2000000000000002</v>
       </c>
@@ -2901,7 +2901,7 @@
       <c r="AB16" s="57"/>
       <c r="AC16" s="57"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="65">
         <v>2.2999999999999998</v>
       </c>
@@ -2921,13 +2921,13 @@
         <v>2</v>
       </c>
       <c r="G17" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="15">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="65">
         <v>2.4</v>
       </c>
@@ -2943,11 +2943,15 @@
       <c r="E18" s="14">
         <v>14</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="F18" s="14">
+        <v>3</v>
+      </c>
+      <c r="G18" s="14">
+        <v>1</v>
+      </c>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="65">
         <v>2.5</v>
       </c>
@@ -2967,7 +2971,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="15"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="65">
         <v>2.6</v>
       </c>
@@ -2987,7 +2991,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="65">
         <v>2.7</v>
       </c>
@@ -3007,7 +3011,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="64">
         <v>3</v>
       </c>
@@ -3021,7 +3025,7 @@
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="65">
         <v>3.1</v>
       </c>
@@ -3035,7 +3039,7 @@
       <c r="G23" s="14"/>
       <c r="H23" s="15"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="65">
         <v>3.2</v>
       </c>
@@ -3049,7 +3053,7 @@
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="65">
         <v>3.3</v>
       </c>
@@ -3063,7 +3067,7 @@
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="65">
         <v>3.4</v>
       </c>
@@ -3077,7 +3081,7 @@
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="65">
         <v>3.5</v>
       </c>
@@ -3091,7 +3095,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="65">
         <v>3.6</v>
       </c>
@@ -3105,7 +3109,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="65">
         <v>3.7</v>
       </c>
@@ -3119,7 +3123,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="65">
         <v>3.8</v>
       </c>
@@ -3133,7 +3137,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="65">
         <v>3.9</v>
       </c>
@@ -3147,7 +3151,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="65" t="s">
         <v>110</v>
       </c>
@@ -3161,7 +3165,7 @@
       <c r="G32" s="14"/>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="65">
         <v>3.11</v>
       </c>
@@ -3175,7 +3179,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="64">
         <v>4</v>
       </c>
@@ -3189,7 +3193,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="65">
         <v>4.0999999999999996</v>
       </c>
@@ -3203,7 +3207,7 @@
       <c r="G35" s="14"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="65">
         <v>4.2</v>
       </c>
@@ -3217,7 +3221,7 @@
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="64">
         <v>5</v>
       </c>
@@ -3231,7 +3235,7 @@
       <c r="G37" s="14"/>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="65">
         <v>5.0999999999999996</v>
       </c>
@@ -3245,7 +3249,7 @@
       <c r="G38" s="14"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="65">
         <v>5.2</v>
       </c>
@@ -3259,7 +3263,7 @@
       <c r="G39" s="14"/>
       <c r="H39" s="15"/>
     </row>
-    <row r="40" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="64">
         <v>6</v>
       </c>
@@ -3273,7 +3277,7 @@
       <c r="G40" s="14"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="65">
         <v>6.1</v>
       </c>
@@ -3287,7 +3291,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="15"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="65">
         <v>6.2</v>
       </c>
@@ -3301,7 +3305,7 @@
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="65">
         <v>6.3</v>
       </c>
@@ -3315,7 +3319,7 @@
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="65">
         <v>6.4</v>
       </c>
@@ -3329,7 +3333,7 @@
       <c r="G44" s="14"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="65">
         <v>6.5</v>
       </c>
@@ -3343,7 +3347,7 @@
       <c r="G45" s="14"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="65">
         <v>6.6</v>
       </c>
@@ -3357,7 +3361,7 @@
       <c r="G46" s="14"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="65">
         <v>6.7</v>
       </c>
@@ -3371,7 +3375,7 @@
       <c r="G47" s="14"/>
       <c r="H47" s="15"/>
     </row>
-    <row r="48" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="64">
         <v>7</v>
       </c>
@@ -3385,7 +3389,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="65">
         <v>7.1</v>
       </c>
@@ -3399,7 +3403,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="65">
         <v>7.2</v>
       </c>
@@ -3413,7 +3417,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="65">
         <v>7.3</v>
       </c>
@@ -3427,7 +3431,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="15"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="65">
         <v>7.4</v>
       </c>
@@ -3441,7 +3445,7 @@
       <c r="G52" s="14"/>
       <c r="H52" s="15"/>
     </row>
-    <row r="53" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="64" t="s">
         <v>127</v>
       </c>
@@ -3455,7 +3459,7 @@
       <c r="G53" s="14"/>
       <c r="H53" s="15"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="65" t="s">
         <v>129</v>
       </c>
@@ -3469,7 +3473,7 @@
       <c r="G54" s="14"/>
       <c r="H54" s="15"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="65" t="s">
         <v>132</v>
       </c>
@@ -3483,7 +3487,7 @@
       <c r="G55" s="14"/>
       <c r="H55" s="15"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="65"/>
       <c r="B56" s="62"/>
       <c r="C56" s="58"/>
@@ -3493,7 +3497,7 @@
       <c r="G56" s="14"/>
       <c r="H56" s="15"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="65"/>
       <c r="B57" s="62"/>
       <c r="C57" s="58"/>
@@ -3503,7 +3507,7 @@
       <c r="G57" s="14"/>
       <c r="H57" s="15"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="65"/>
       <c r="B58" s="62"/>
       <c r="C58" s="58"/>
@@ -3513,7 +3517,7 @@
       <c r="G58" s="14"/>
       <c r="H58" s="15"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="65"/>
       <c r="B59" s="62"/>
       <c r="C59" s="58"/>
@@ -3523,7 +3527,7 @@
       <c r="G59" s="14"/>
       <c r="H59" s="15"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="65"/>
       <c r="B60" s="62"/>
       <c r="C60" s="58"/>
@@ -3533,26 +3537,26 @@
       <c r="G60" s="14"/>
       <c r="H60" s="15"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="41"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="41"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="41"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>53</v>
       </c>
@@ -3615,15 +3619,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>15</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:colOff>63500</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>15</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3652,14 +3656,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.875" customWidth="1"/>
-    <col min="2" max="2" width="125.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="125.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
         <v>45</v>
       </c>
@@ -3670,7 +3674,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="52" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="51">
         <v>1.1000000000000001</v>
       </c>
@@ -3679,44 +3683,44 @@
       </c>
       <c r="C3" s="51"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="17"/>
       <c r="B4" s="47"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="47"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="48"/>
       <c r="B6" s="47"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="47"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="48"/>
       <c r="B8" s="47"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="47"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="48"/>
       <c r="B10" s="47"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="48"/>
       <c r="B11" s="47"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="48"/>
       <c r="B12" s="47"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
       <c r="B21" s="42"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update get_info for Student
</commit_message>
<xml_diff>
--- a/planner.xlsx
+++ b/planner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CF72CF-E532-43AC-A524-138EC7A252C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B814C1-4B2F-421B-829D-E0F3C4D60F54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3960" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -1255,14 +1255,14 @@
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Đầu đề 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -2153,12 +2153,12 @@
   </sheetPr>
   <dimension ref="A1:BN68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="9" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2245,7 +2245,7 @@
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
     </row>
-    <row r="4" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="32" t="s">
@@ -2267,82 +2267,228 @@
       <c r="J4" s="45">
         <v>43940</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
+      <c r="K4" s="45">
+        <f>J4+1</f>
+        <v>43941</v>
+      </c>
+      <c r="L4" s="45">
+        <f t="shared" ref="L4:BN4" si="0">K4+1</f>
+        <v>43942</v>
+      </c>
+      <c r="M4" s="45">
+        <f t="shared" si="0"/>
+        <v>43943</v>
+      </c>
+      <c r="N4" s="45">
+        <f t="shared" si="0"/>
+        <v>43944</v>
+      </c>
+      <c r="O4" s="45">
+        <f t="shared" si="0"/>
+        <v>43945</v>
+      </c>
+      <c r="P4" s="45">
+        <f t="shared" si="0"/>
+        <v>43946</v>
+      </c>
       <c r="Q4" s="45">
-        <f>J4+7</f>
+        <f t="shared" si="0"/>
         <v>43947</v>
       </c>
-      <c r="R4" s="35"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
+      <c r="R4" s="45">
+        <f t="shared" si="0"/>
+        <v>43948</v>
+      </c>
+      <c r="S4" s="45">
+        <f t="shared" si="0"/>
+        <v>43949</v>
+      </c>
+      <c r="T4" s="45">
+        <f t="shared" si="0"/>
+        <v>43950</v>
+      </c>
+      <c r="U4" s="45">
+        <f t="shared" si="0"/>
+        <v>43951</v>
+      </c>
+      <c r="V4" s="45">
+        <f t="shared" si="0"/>
+        <v>43952</v>
+      </c>
+      <c r="W4" s="45">
+        <f t="shared" si="0"/>
+        <v>43953</v>
+      </c>
       <c r="X4" s="45">
-        <f t="shared" ref="X4" si="0">Q4+7</f>
+        <f t="shared" si="0"/>
         <v>43954</v>
       </c>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="1"/>
+      <c r="Y4" s="45">
+        <f t="shared" si="0"/>
+        <v>43955</v>
+      </c>
+      <c r="Z4" s="45">
+        <f t="shared" si="0"/>
+        <v>43956</v>
+      </c>
+      <c r="AA4" s="45">
+        <f t="shared" si="0"/>
+        <v>43957</v>
+      </c>
+      <c r="AB4" s="45">
+        <f t="shared" si="0"/>
+        <v>43958</v>
+      </c>
+      <c r="AC4" s="45">
+        <f t="shared" si="0"/>
+        <v>43959</v>
+      </c>
+      <c r="AD4" s="45">
+        <f t="shared" si="0"/>
+        <v>43960</v>
+      </c>
       <c r="AE4" s="45">
-        <f t="shared" ref="AE4" si="1">X4+7</f>
+        <f t="shared" si="0"/>
         <v>43961</v>
       </c>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="36"/>
-      <c r="AH4" s="36"/>
-      <c r="AI4" s="36"/>
-      <c r="AJ4" s="36"/>
-      <c r="AK4" s="1"/>
+      <c r="AF4" s="45">
+        <f t="shared" si="0"/>
+        <v>43962</v>
+      </c>
+      <c r="AG4" s="45">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="AH4" s="45">
+        <f t="shared" si="0"/>
+        <v>43964</v>
+      </c>
+      <c r="AI4" s="45">
+        <f t="shared" si="0"/>
+        <v>43965</v>
+      </c>
+      <c r="AJ4" s="45">
+        <f t="shared" si="0"/>
+        <v>43966</v>
+      </c>
+      <c r="AK4" s="45">
+        <f t="shared" si="0"/>
+        <v>43967</v>
+      </c>
       <c r="AL4" s="45">
-        <f t="shared" ref="AL4" si="2">AE4+7</f>
+        <f t="shared" si="0"/>
         <v>43968</v>
       </c>
-      <c r="AM4" s="35"/>
-      <c r="AN4" s="36"/>
-      <c r="AO4" s="36"/>
-      <c r="AP4" s="36"/>
-      <c r="AQ4" s="36"/>
-      <c r="AR4" s="1"/>
+      <c r="AM4" s="45">
+        <f t="shared" si="0"/>
+        <v>43969</v>
+      </c>
+      <c r="AN4" s="45">
+        <f t="shared" si="0"/>
+        <v>43970</v>
+      </c>
+      <c r="AO4" s="45">
+        <f t="shared" si="0"/>
+        <v>43971</v>
+      </c>
+      <c r="AP4" s="45">
+        <f t="shared" si="0"/>
+        <v>43972</v>
+      </c>
+      <c r="AQ4" s="45">
+        <f t="shared" si="0"/>
+        <v>43973</v>
+      </c>
+      <c r="AR4" s="45">
+        <f t="shared" si="0"/>
+        <v>43974</v>
+      </c>
       <c r="AS4" s="45">
-        <f t="shared" ref="AS4" si="3">AL4+7</f>
+        <f t="shared" si="0"/>
         <v>43975</v>
       </c>
-      <c r="AT4" s="35"/>
-      <c r="AU4" s="36"/>
-      <c r="AV4" s="36"/>
-      <c r="AW4" s="36"/>
-      <c r="AX4" s="36"/>
-      <c r="AY4" s="1"/>
+      <c r="AT4" s="45">
+        <f t="shared" si="0"/>
+        <v>43976</v>
+      </c>
+      <c r="AU4" s="45">
+        <f t="shared" si="0"/>
+        <v>43977</v>
+      </c>
+      <c r="AV4" s="45">
+        <f t="shared" si="0"/>
+        <v>43978</v>
+      </c>
+      <c r="AW4" s="45">
+        <f t="shared" si="0"/>
+        <v>43979</v>
+      </c>
+      <c r="AX4" s="45">
+        <f t="shared" si="0"/>
+        <v>43980</v>
+      </c>
+      <c r="AY4" s="45">
+        <f t="shared" si="0"/>
+        <v>43981</v>
+      </c>
       <c r="AZ4" s="45">
-        <f t="shared" ref="AZ4" si="4">AS4+7</f>
+        <f t="shared" si="0"/>
         <v>43982</v>
       </c>
-      <c r="BA4" s="35"/>
-      <c r="BB4" s="36"/>
-      <c r="BC4" s="36"/>
-      <c r="BD4" s="36"/>
-      <c r="BE4" s="36"/>
-      <c r="BF4" s="1"/>
+      <c r="BA4" s="45">
+        <f t="shared" si="0"/>
+        <v>43983</v>
+      </c>
+      <c r="BB4" s="45">
+        <f t="shared" si="0"/>
+        <v>43984</v>
+      </c>
+      <c r="BC4" s="45">
+        <f t="shared" si="0"/>
+        <v>43985</v>
+      </c>
+      <c r="BD4" s="45">
+        <f t="shared" si="0"/>
+        <v>43986</v>
+      </c>
+      <c r="BE4" s="45">
+        <f t="shared" si="0"/>
+        <v>43987</v>
+      </c>
+      <c r="BF4" s="45">
+        <f t="shared" si="0"/>
+        <v>43988</v>
+      </c>
       <c r="BG4" s="45">
-        <f t="shared" ref="BG4" si="5">AZ4+7</f>
+        <f t="shared" si="0"/>
         <v>43989</v>
       </c>
-      <c r="BH4" s="35"/>
-      <c r="BI4" s="36"/>
-      <c r="BJ4" s="36"/>
-      <c r="BK4" s="36"/>
-      <c r="BL4" s="36"/>
-      <c r="BM4" s="1"/>
+      <c r="BH4" s="45">
+        <f t="shared" si="0"/>
+        <v>43990</v>
+      </c>
+      <c r="BI4" s="45">
+        <f t="shared" si="0"/>
+        <v>43991</v>
+      </c>
+      <c r="BJ4" s="45">
+        <f t="shared" si="0"/>
+        <v>43992</v>
+      </c>
+      <c r="BK4" s="45">
+        <f t="shared" si="0"/>
+        <v>43993</v>
+      </c>
+      <c r="BL4" s="45">
+        <f t="shared" si="0"/>
+        <v>43994</v>
+      </c>
+      <c r="BM4" s="45">
+        <f t="shared" si="0"/>
+        <v>43995</v>
+      </c>
       <c r="BN4" s="45">
-        <f t="shared" ref="BN4" si="6">BG4+7</f>
+        <f t="shared" si="0"/>
         <v>43996</v>
       </c>
     </row>
@@ -2722,10 +2868,10 @@
         <v>2</v>
       </c>
       <c r="G9" s="14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H9" s="15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.25">
@@ -2748,7 +2894,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H10" s="15">
         <v>0.5</v>

</xml_diff>

<commit_message>
fix comment for change_password function
</commit_message>
<xml_diff>
--- a/planner.xlsx
+++ b/planner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AC243D-BB4B-4F8A-99D6-BE53BF65299A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7E305F-1C1D-4ED8-8262-13A77B846A74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1253,14 +1255,14 @@
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Đầu đề 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -1498,15 +1500,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>15</xdr:col>
           <xdr:colOff>190500</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1794,16 +1796,16 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="52.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.875" customWidth="1"/>
+    <col min="2" max="2" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="52.125" customWidth="1"/>
+    <col min="4" max="4" width="14.875" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>14</v>
       </c>
@@ -1815,7 +1817,7 @@
       <c r="G1" s="69"/>
       <c r="H1" s="69"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="69"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -1825,7 +1827,7 @@
       <c r="G2" s="69"/>
       <c r="H2" s="69"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="69"/>
       <c r="B3" s="69"/>
       <c r="C3" s="69"/>
@@ -1835,7 +1837,7 @@
       <c r="G3" s="69"/>
       <c r="H3" s="69"/>
     </row>
-    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>32</v>
       </c>
@@ -1843,7 +1845,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>33</v>
       </c>
@@ -1851,7 +1853,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
@@ -1859,7 +1861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>15</v>
       </c>
@@ -1876,7 +1878,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>17</v>
       </c>
@@ -1887,7 +1889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>18</v>
       </c>
@@ -1898,7 +1900,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>19</v>
       </c>
@@ -1908,7 +1910,7 @@
       <c r="E13" s="27"/>
       <c r="F13" s="26"/>
     </row>
-    <row r="14" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>20</v>
       </c>
@@ -1917,7 +1919,7 @@
       </c>
       <c r="F14" s="26"/>
     </row>
-    <row r="15" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
         <v>21</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>22</v>
       </c>
@@ -1953,15 +1955,15 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.625" customWidth="1"/>
+    <col min="3" max="3" width="27.625" customWidth="1"/>
+    <col min="4" max="4" width="21.125" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>34</v>
       </c>
@@ -1971,7 +1973,7 @@
       <c r="E1" s="69"/>
       <c r="F1" s="69"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="69"/>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -1979,7 +1981,7 @@
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
     </row>
-    <row r="3" spans="1:6" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="69"/>
       <c r="B3" s="69"/>
       <c r="C3" s="69"/>
@@ -1987,7 +1989,7 @@
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>35</v>
       </c>
@@ -1995,10 +1997,10 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>36</v>
       </c>
@@ -2012,7 +2014,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" s="67" t="s">
         <v>99</v>
@@ -2024,7 +2026,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="67" t="s">
         <v>100</v>
@@ -2036,7 +2038,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="67" t="s">
         <v>101</v>
@@ -2048,7 +2050,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="67" t="s">
         <v>102</v>
@@ -2060,16 +2062,16 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="67"/>
       <c r="D11" s="68"/>
       <c r="E11" s="67"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>37</v>
       </c>
@@ -2080,7 +2082,7 @@
         <v>43940</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>38</v>
       </c>
@@ -2089,41 +2091,41 @@
       </c>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="28"/>
     </row>
-    <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" ht="21" x14ac:dyDescent="0.25">
       <c r="C21" s="50" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C22" s="46" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C23" s="46" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C24" s="46" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C25" s="46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="3:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="C27" s="54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="3:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="C28" s="54" t="s">
         <v>97</v>
       </c>
@@ -2156,25 +2158,25 @@
       <selection activeCell="K7" sqref="K7"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="40" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="41.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="4.109375" style="1" customWidth="1"/>
-    <col min="10" max="29" width="7.6640625" style="1" customWidth="1"/>
-    <col min="30" max="66" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="4.125" style="1" customWidth="1"/>
+    <col min="10" max="29" width="7.625" style="1" customWidth="1"/>
+    <col min="30" max="66" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:66" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
@@ -2185,7 +2187,7 @@
       <c r="G1" s="70"/>
       <c r="H1" s="70"/>
     </row>
-    <row r="2" spans="1:66" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:66" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -2229,7 +2231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:66" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:66" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="70"/>
       <c r="C3" s="70"/>
       <c r="D3" s="70"/>
@@ -2243,7 +2245,7 @@
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
     </row>
-    <row r="4" spans="1:66" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="32" t="s">
@@ -2490,7 +2492,7 @@
         <v>43996</v>
       </c>
     </row>
-    <row r="5" spans="1:66" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
         <v>45</v>
       </c>
@@ -2576,7 +2578,7 @@
       <c r="BM5" s="36"/>
       <c r="BN5" s="37"/>
     </row>
-    <row r="6" spans="1:66" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
       <c r="D6" s="38" t="s">
@@ -2765,7 +2767,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:66" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="59"/>
       <c r="C7" s="60"/>
       <c r="D7" s="60"/>
@@ -2832,7 +2834,7 @@
       <c r="BM7" s="3"/>
       <c r="BN7" s="3"/>
     </row>
-    <row r="8" spans="1:66" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:66" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="64">
         <v>1</v>
       </c>
@@ -2846,7 +2848,7 @@
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:66" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A9" s="65">
         <v>1.1000000000000001</v>
       </c>
@@ -2866,13 +2868,13 @@
         <v>2</v>
       </c>
       <c r="G9" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H9" s="15">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" s="65">
         <v>1.2</v>
       </c>
@@ -2892,13 +2894,13 @@
         <v>2</v>
       </c>
       <c r="G10" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H10" s="15">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" s="65">
         <v>1.3</v>
       </c>
@@ -2924,7 +2926,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A12" s="65">
         <v>1.4</v>
       </c>
@@ -2950,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A13" s="65">
         <v>1.5</v>
       </c>
@@ -2976,7 +2978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:66" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:66" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A14" s="64">
         <v>2</v>
       </c>
@@ -2990,7 +2992,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A15" s="65">
         <v>2.1</v>
       </c>
@@ -3016,7 +3018,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:66" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:66" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="66">
         <v>2.2000000000000002</v>
       </c>
@@ -3057,7 +3059,7 @@
       <c r="AB16" s="57"/>
       <c r="AC16" s="57"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="65">
         <v>2.2999999999999998</v>
       </c>
@@ -3083,7 +3085,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="65">
         <v>2.4</v>
       </c>
@@ -3109,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="65">
         <v>2.5</v>
       </c>
@@ -3129,7 +3131,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="15"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="65">
         <v>2.6</v>
       </c>
@@ -3149,7 +3151,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="65">
         <v>2.7</v>
       </c>
@@ -3169,7 +3171,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A22" s="64">
         <v>3</v>
       </c>
@@ -3183,7 +3185,7 @@
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="65">
         <v>3.1</v>
       </c>
@@ -3197,7 +3199,7 @@
       <c r="G23" s="14"/>
       <c r="H23" s="15"/>
     </row>
-    <row r="24" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="65">
         <v>3.2</v>
       </c>
@@ -3211,7 +3213,7 @@
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="65">
         <v>3.3</v>
       </c>
@@ -3225,7 +3227,7 @@
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="65">
         <v>3.4</v>
       </c>
@@ -3239,7 +3241,7 @@
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="65">
         <v>3.5</v>
       </c>
@@ -3253,7 +3255,7 @@
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="65">
         <v>3.6</v>
       </c>
@@ -3267,7 +3269,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="65">
         <v>3.7</v>
       </c>
@@ -3281,7 +3283,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="65">
         <v>3.8</v>
       </c>
@@ -3295,7 +3297,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="65">
         <v>3.9</v>
       </c>
@@ -3309,7 +3311,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="65" t="s">
         <v>110</v>
       </c>
@@ -3323,7 +3325,7 @@
       <c r="G32" s="14"/>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="65">
         <v>3.11</v>
       </c>
@@ -3337,7 +3339,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A34" s="64">
         <v>4</v>
       </c>
@@ -3351,7 +3353,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="65">
         <v>4.0999999999999996</v>
       </c>
@@ -3365,7 +3367,7 @@
       <c r="G35" s="14"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="65">
         <v>4.2</v>
       </c>
@@ -3379,7 +3381,7 @@
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A37" s="64">
         <v>5</v>
       </c>
@@ -3393,7 +3395,7 @@
       <c r="G37" s="14"/>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="65">
         <v>5.0999999999999996</v>
       </c>
@@ -3407,7 +3409,7 @@
       <c r="G38" s="14"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="65">
         <v>5.2</v>
       </c>
@@ -3421,7 +3423,7 @@
       <c r="G39" s="14"/>
       <c r="H39" s="15"/>
     </row>
-    <row r="40" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A40" s="64">
         <v>6</v>
       </c>
@@ -3435,7 +3437,7 @@
       <c r="G40" s="14"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="65">
         <v>6.1</v>
       </c>
@@ -3449,7 +3451,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="15"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="65">
         <v>6.2</v>
       </c>
@@ -3463,7 +3465,7 @@
       <c r="G42" s="14"/>
       <c r="H42" s="15"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="65">
         <v>6.3</v>
       </c>
@@ -3477,7 +3479,7 @@
       <c r="G43" s="14"/>
       <c r="H43" s="15"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="65">
         <v>6.4</v>
       </c>
@@ -3491,7 +3493,7 @@
       <c r="G44" s="14"/>
       <c r="H44" s="15"/>
     </row>
-    <row r="45" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="65">
         <v>6.5</v>
       </c>
@@ -3505,7 +3507,7 @@
       <c r="G45" s="14"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="65">
         <v>6.6</v>
       </c>
@@ -3519,7 +3521,7 @@
       <c r="G46" s="14"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="65">
         <v>6.7</v>
       </c>
@@ -3533,7 +3535,7 @@
       <c r="G47" s="14"/>
       <c r="H47" s="15"/>
     </row>
-    <row r="48" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A48" s="64">
         <v>7</v>
       </c>
@@ -3547,7 +3549,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="65">
         <v>7.1</v>
       </c>
@@ -3561,7 +3563,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="65">
         <v>7.2</v>
       </c>
@@ -3575,7 +3577,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="65">
         <v>7.3</v>
       </c>
@@ -3589,7 +3591,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="15"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="65">
         <v>7.4</v>
       </c>
@@ -3603,7 +3605,7 @@
       <c r="G52" s="14"/>
       <c r="H52" s="15"/>
     </row>
-    <row r="53" spans="1:8" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="64" t="s">
         <v>127</v>
       </c>
@@ -3617,7 +3619,7 @@
       <c r="G53" s="14"/>
       <c r="H53" s="15"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="65" t="s">
         <v>129</v>
       </c>
@@ -3631,7 +3633,7 @@
       <c r="G54" s="14"/>
       <c r="H54" s="15"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="65" t="s">
         <v>132</v>
       </c>
@@ -3645,7 +3647,7 @@
       <c r="G55" s="14"/>
       <c r="H55" s="15"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="65"/>
       <c r="B56" s="62"/>
       <c r="C56" s="58"/>
@@ -3655,7 +3657,7 @@
       <c r="G56" s="14"/>
       <c r="H56" s="15"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="65"/>
       <c r="B57" s="62"/>
       <c r="C57" s="58"/>
@@ -3665,7 +3667,7 @@
       <c r="G57" s="14"/>
       <c r="H57" s="15"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="65"/>
       <c r="B58" s="62"/>
       <c r="C58" s="58"/>
@@ -3675,7 +3677,7 @@
       <c r="G58" s="14"/>
       <c r="H58" s="15"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="65"/>
       <c r="B59" s="62"/>
       <c r="C59" s="58"/>
@@ -3685,7 +3687,7 @@
       <c r="G59" s="14"/>
       <c r="H59" s="15"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="65"/>
       <c r="B60" s="62"/>
       <c r="C60" s="58"/>
@@ -3695,26 +3697,26 @@
       <c r="G60" s="14"/>
       <c r="H60" s="15"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="41"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="41"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="41"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
         <v>53</v>
       </c>
@@ -3777,15 +3779,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>15</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
+                    <xdr:colOff>66675</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>15</xdr:col>
                     <xdr:colOff>190500</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3814,14 +3816,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="125.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="125.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>45</v>
       </c>
@@ -3832,7 +3834,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="52" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="52" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="51">
         <v>1.1000000000000001</v>
       </c>
@@ -3841,44 +3843,44 @@
       </c>
       <c r="C3" s="51"/>
     </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="47"/>
     </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
     </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="48"/>
       <c r="B6" s="47"/>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="47"/>
     </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="48"/>
       <c r="B8" s="47"/>
     </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="47"/>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="47"/>
     </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
       <c r="B11" s="47"/>
     </row>
-    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
       <c r="B12" s="47"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="42"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
complete login, profile, ... functions
</commit_message>
<xml_diff>
--- a/planner.xlsx
+++ b/planner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCAB3BE-02B5-4A23-879E-B61AB3A90092}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34B587B-6258-4697-BFD9-74FD5F455D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="135">
   <si>
     <t>Project Planner Guide</t>
   </si>
@@ -603,6 +603,9 @@
   <si>
     <t>Staff login done (1/3)</t>
   </si>
+  <si>
+    <t>change into Data Abstract</t>
+  </si>
 </sst>
 </file>
 
@@ -613,7 +616,7 @@
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="dd\ mmm\ yy"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -886,6 +889,18 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1044,7 +1059,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1189,9 +1204,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1245,18 +1257,24 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Đầu đề 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Siêu kết nối" xfId="8" builtinId="8"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -1791,36 +1809,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="6" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
@@ -1949,30 +1967,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:6" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
@@ -2001,57 +2019,57 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="16"/>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="65" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="65" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="16"/>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="65" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="67" t="s">
+      <c r="D10" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="65" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="16"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="66"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="65"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="16"/>
@@ -2106,12 +2124,12 @@
       </c>
     </row>
     <row r="27" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="52" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="28" spans="3:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="C28" s="53" t="s">
+      <c r="C28" s="52" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2139,10 +2157,10 @@
   <dimension ref="A1:BN68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="9" ySplit="6" topLeftCell="S7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K7" sqref="K7"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2161,24 +2179,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:66" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
       <c r="J2" s="7" t="s">
         <v>57</v>
       </c>
@@ -2191,11 +2209,11 @@
       </c>
       <c r="P2" s="7"/>
       <c r="R2" s="9"/>
-      <c r="S2" s="68" t="s">
+      <c r="S2" s="67" t="s">
         <v>58</v>
       </c>
       <c r="U2" s="10"/>
-      <c r="V2" s="68" t="s">
+      <c r="V2" s="67" t="s">
         <v>59</v>
       </c>
       <c r="Y2" s="11"/>
@@ -2216,13 +2234,13 @@
       </c>
     </row>
     <row r="3" spans="1:66" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
@@ -2752,14 +2770,14 @@
       </c>
     </row>
     <row r="7" spans="1:66" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="60"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="59"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -2819,13 +2837,13 @@
       <c r="BN7" s="3"/>
     </row>
     <row r="8" spans="1:66" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="63">
+      <c r="A8" s="62">
         <v>1</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="57"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -2833,13 +2851,13 @@
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A9" s="64">
+      <c r="A9" s="63">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="56" t="s">
         <v>77</v>
       </c>
       <c r="D9" s="14">
@@ -2852,20 +2870,20 @@
         <v>2</v>
       </c>
       <c r="G9" s="14">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H9" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A10" s="64">
+      <c r="A10" s="63">
         <v>1.2</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="56" t="s">
         <v>77</v>
       </c>
       <c r="D10" s="14">
@@ -2878,20 +2896,20 @@
         <v>2</v>
       </c>
       <c r="G10" s="14">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H10" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A11" s="64">
+      <c r="A11" s="63">
         <v>1.3</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="56" t="s">
         <v>77</v>
       </c>
       <c r="D11" s="14">
@@ -2904,20 +2922,20 @@
         <v>6</v>
       </c>
       <c r="G11" s="14">
+        <v>8</v>
+      </c>
+      <c r="H11" s="15">
         <v>1</v>
       </c>
-      <c r="H11" s="15">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A12" s="64">
+      <c r="A12" s="63">
         <v>1.4</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="56" t="s">
         <v>77</v>
       </c>
       <c r="D12" s="14">
@@ -2937,13 +2955,13 @@
       </c>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A13" s="64">
+      <c r="A13" s="63">
         <v>1.5</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="56" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="14">
@@ -2963,13 +2981,13 @@
       </c>
     </row>
     <row r="14" spans="1:66" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="63">
+      <c r="A14" s="62">
         <v>2</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -2977,13 +2995,13 @@
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A15" s="64">
+      <c r="A15" s="63">
         <v>2.1</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="56" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="14">
@@ -3003,13 +3021,13 @@
       </c>
     </row>
     <row r="16" spans="1:66" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65">
+      <c r="A16" s="64">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="56" t="s">
         <v>84</v>
       </c>
       <c r="D16" s="14">
@@ -3018,39 +3036,39 @@
       <c r="E16" s="14">
         <v>14</v>
       </c>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
-      <c r="Y16" s="56"/>
-      <c r="Z16" s="56"/>
-      <c r="AA16" s="56"/>
-      <c r="AB16" s="56"/>
-      <c r="AC16" s="56"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
+      <c r="Y16" s="55"/>
+      <c r="Z16" s="55"/>
+      <c r="AA16" s="55"/>
+      <c r="AB16" s="55"/>
+      <c r="AC16" s="55"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="64">
+      <c r="A17" s="63">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="56" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="14">
@@ -3070,13 +3088,13 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="64">
+      <c r="A18" s="63">
         <v>2.4</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="56" t="s">
         <v>87</v>
       </c>
       <c r="D18" s="14">
@@ -3096,13 +3114,13 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="64">
+      <c r="A19" s="63">
         <v>2.5</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="56" t="s">
         <v>90</v>
       </c>
       <c r="D19" s="14">
@@ -3122,13 +3140,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="64">
+      <c r="A20" s="63">
         <v>2.6</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="56" t="s">
         <v>90</v>
       </c>
       <c r="D20" s="14">
@@ -3148,13 +3166,13 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="64">
+      <c r="A21" s="63">
         <v>2.7</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="56" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="14">
@@ -3174,13 +3192,13 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="63">
+      <c r="A22" s="62">
         <v>3</v>
       </c>
       <c r="B22" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="57"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
@@ -3188,111 +3206,155 @@
       <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="64">
+      <c r="A23" s="63">
         <v>3.1</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="C23" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="14">
+        <v>16</v>
+      </c>
+      <c r="E23" s="14">
+        <v>14</v>
+      </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="64">
+      <c r="A24" s="63">
         <v>3.2</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="C24" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="14">
+        <v>16</v>
+      </c>
+      <c r="E24" s="14">
+        <v>14</v>
+      </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="64">
+      <c r="A25" s="63">
         <v>3.3</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="C25" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="14">
+        <v>16</v>
+      </c>
+      <c r="E25" s="14">
+        <v>14</v>
+      </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="64">
+      <c r="A26" s="63">
         <v>3.4</v>
       </c>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="C26" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="14">
+        <v>16</v>
+      </c>
+      <c r="E26" s="14">
+        <v>14</v>
+      </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="64">
+      <c r="A27" s="63">
         <v>3.5</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="C27" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="14">
+        <v>16</v>
+      </c>
+      <c r="E27" s="14">
+        <v>14</v>
+      </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="64">
+      <c r="A28" s="63">
         <v>3.6</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="C28" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="14">
+        <v>16</v>
+      </c>
+      <c r="E28" s="14">
+        <v>14</v>
+      </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="64">
+      <c r="A29" s="63">
         <v>3.7</v>
       </c>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="C29" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="14">
+        <v>16</v>
+      </c>
+      <c r="E29" s="14">
+        <v>14</v>
+      </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="64">
+      <c r="A30" s="63">
         <v>3.8</v>
       </c>
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="57"/>
+      <c r="C30" s="56" t="s">
+        <v>90</v>
+      </c>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
@@ -3300,13 +3362,15 @@
       <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="64">
+      <c r="A31" s="63">
         <v>3.9</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="57"/>
+      <c r="C31" s="56" t="s">
+        <v>87</v>
+      </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
@@ -3314,13 +3378,15 @@
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="57"/>
+      <c r="C32" s="56" t="s">
+        <v>84</v>
+      </c>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
@@ -3328,27 +3394,33 @@
       <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="64">
+      <c r="A33" s="63">
         <v>3.11</v>
       </c>
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="57"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
+      <c r="C33" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="14">
+        <v>16</v>
+      </c>
+      <c r="E33" s="14">
+        <v>14</v>
+      </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
     </row>
     <row r="34" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="63">
+      <c r="A34" s="62">
         <v>4</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="57"/>
+      <c r="C34" s="56"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
@@ -3356,13 +3428,13 @@
       <c r="H34" s="15"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="64">
+      <c r="A35" s="63">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="57"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
@@ -3370,13 +3442,13 @@
       <c r="H35" s="15"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="64">
+      <c r="A36" s="63">
         <v>4.2</v>
       </c>
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="57"/>
+      <c r="C36" s="56"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
@@ -3384,13 +3456,13 @@
       <c r="H36" s="15"/>
     </row>
     <row r="37" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="63">
+      <c r="A37" s="62">
         <v>5</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="57"/>
+      <c r="C37" s="56"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
@@ -3398,13 +3470,13 @@
       <c r="H37" s="15"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="64">
+      <c r="A38" s="63">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B38" s="61" t="s">
+      <c r="B38" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="57"/>
+      <c r="C38" s="56"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
@@ -3412,13 +3484,13 @@
       <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="64">
+      <c r="A39" s="63">
         <v>5.2</v>
       </c>
-      <c r="B39" s="61" t="s">
+      <c r="B39" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="57"/>
+      <c r="C39" s="56"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -3426,13 +3498,13 @@
       <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="63">
+      <c r="A40" s="62">
         <v>6</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="57"/>
+      <c r="C40" s="56"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
@@ -3440,13 +3512,13 @@
       <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="64">
+      <c r="A41" s="63">
         <v>6.1</v>
       </c>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="57"/>
+      <c r="C41" s="56"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
@@ -3454,13 +3526,13 @@
       <c r="H41" s="15"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="64">
+      <c r="A42" s="63">
         <v>6.2</v>
       </c>
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="57"/>
+      <c r="C42" s="56"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
@@ -3468,13 +3540,13 @@
       <c r="H42" s="15"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="64">
+      <c r="A43" s="63">
         <v>6.3</v>
       </c>
-      <c r="B43" s="61" t="s">
+      <c r="B43" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="57"/>
+      <c r="C43" s="56"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
@@ -3482,13 +3554,13 @@
       <c r="H43" s="15"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="64">
+      <c r="A44" s="63">
         <v>6.4</v>
       </c>
-      <c r="B44" s="61" t="s">
+      <c r="B44" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="57"/>
+      <c r="C44" s="56"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
@@ -3496,13 +3568,13 @@
       <c r="H44" s="15"/>
     </row>
     <row r="45" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="64">
+      <c r="A45" s="63">
         <v>6.5</v>
       </c>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="57"/>
+      <c r="C45" s="56"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
@@ -3510,13 +3582,13 @@
       <c r="H45" s="15"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="64">
+      <c r="A46" s="63">
         <v>6.6</v>
       </c>
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="57"/>
+      <c r="C46" s="56"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
@@ -3524,13 +3596,13 @@
       <c r="H46" s="15"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="64">
+      <c r="A47" s="63">
         <v>6.7</v>
       </c>
-      <c r="B47" s="61" t="s">
+      <c r="B47" s="60" t="s">
         <v>116</v>
       </c>
-      <c r="C47" s="57"/>
+      <c r="C47" s="56"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
@@ -3538,13 +3610,13 @@
       <c r="H47" s="15"/>
     </row>
     <row r="48" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="63">
+      <c r="A48" s="62">
         <v>7</v>
       </c>
       <c r="B48" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="C48" s="57"/>
+      <c r="C48" s="56"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
@@ -3552,13 +3624,13 @@
       <c r="H48" s="15"/>
     </row>
     <row r="49" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="64">
+      <c r="A49" s="63">
         <v>7.1</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="57"/>
+      <c r="C49" s="56"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
@@ -3566,13 +3638,13 @@
       <c r="H49" s="15"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="64">
+      <c r="A50" s="63">
         <v>7.2</v>
       </c>
-      <c r="B50" s="61" t="s">
+      <c r="B50" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="C50" s="57"/>
+      <c r="C50" s="56"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
@@ -3580,13 +3652,13 @@
       <c r="H50" s="15"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="64">
+      <c r="A51" s="63">
         <v>7.3</v>
       </c>
-      <c r="B51" s="61" t="s">
+      <c r="B51" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="57"/>
+      <c r="C51" s="56"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
@@ -3594,13 +3666,13 @@
       <c r="H51" s="15"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="64">
+      <c r="A52" s="63">
         <v>7.4</v>
       </c>
-      <c r="B52" s="61" t="s">
+      <c r="B52" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="C52" s="57"/>
+      <c r="C52" s="56"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
@@ -3608,13 +3680,13 @@
       <c r="H52" s="15"/>
     </row>
     <row r="53" spans="1:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="63" t="s">
+      <c r="A53" s="62" t="s">
         <v>122</v>
       </c>
       <c r="B53" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="57"/>
+      <c r="C53" s="56"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14"/>
@@ -3622,13 +3694,13 @@
       <c r="H53" s="15"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="64" t="s">
+      <c r="A54" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="C54" s="57"/>
+      <c r="C54" s="56"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -3636,13 +3708,13 @@
       <c r="H54" s="15"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="64" t="s">
+      <c r="A55" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="61" t="s">
+      <c r="B55" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C55" s="57"/>
+      <c r="C55" s="56"/>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
@@ -3650,9 +3722,9 @@
       <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="64"/>
-      <c r="B56" s="61"/>
-      <c r="C56" s="57"/>
+      <c r="A56" s="63"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="56"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
@@ -3660,9 +3732,9 @@
       <c r="H56" s="15"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="64"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="57"/>
+      <c r="A57" s="63"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="56"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="14"/>
@@ -3670,9 +3742,9 @@
       <c r="H57" s="15"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="64"/>
-      <c r="B58" s="61"/>
-      <c r="C58" s="57"/>
+      <c r="A58" s="63"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="56"/>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="14"/>
@@ -3680,9 +3752,9 @@
       <c r="H58" s="15"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="64"/>
-      <c r="B59" s="61"/>
-      <c r="C59" s="57"/>
+      <c r="A59" s="63"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="56"/>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -3690,9 +3762,9 @@
       <c r="H59" s="15"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="64"/>
-      <c r="B60" s="61"/>
-      <c r="C60" s="57"/>
+      <c r="A60" s="63"/>
+      <c r="B60" s="60"/>
+      <c r="C60" s="56"/>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="14"/>
@@ -3785,8 +3857,8 @@
   </sheetPr>
   <dimension ref="A2:C24"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="B1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3808,17 +3880,21 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="51" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="50">
+      <c r="A3" s="70">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="71" t="s">
         <v>133</v>
       </c>
       <c r="C3" s="50"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="16">
+        <v>0</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="46"/>

</xml_diff>